<commit_message>
Minor changes to udp connection
</commit_message>
<xml_diff>
--- a/lib/Vortex127.xlsx
+++ b/lib/Vortex127.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C497F80-8990-476B-846C-946394FBE403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B159AA-C453-4FFE-9B70-EF2D620D216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Graph #</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>PIP</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1258,7 @@
   <dimension ref="A2:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,10 +2216,10 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B32" s="58" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="D32" s="72" t="s">
         <v>22</v>
@@ -2690,20 +2693,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2726,6 +2729,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2740,12 +2751,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed bug with combo box
</commit_message>
<xml_diff>
--- a/lib/Vortex127.xlsx
+++ b/lib/Vortex127.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Sailproj\SailProjGit\SAILcode\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B159AA-C453-4FFE-9B70-EF2D620D216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C857CFB1-FA61-47F4-BD47-2025AE35EEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>Graph #</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>PIP</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1255,7 @@
   <dimension ref="A2:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1299,7 @@
         <v>55</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>34</v>
@@ -2216,10 +2213,10 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B32" s="58" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="D32" s="72" t="s">
         <v>22</v>

</xml_diff>